<commit_message>
Updated categories in Expenses.xlsx
subsetted data into Expenses, Income, and Investements
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffgood/Desktop/FI/Expenses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffgood/Desktop/R_Studio_Projects/Financial_Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910D6CAB-A14E-4745-88BE-C6E2CBAF81FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35595B41-A7EA-E54C-AA53-CD96E62AA944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="1000" windowWidth="27380" windowHeight="15800" xr2:uid="{D9F47917-7B20-384C-878F-0D08681ABD47}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId4"/>
+    <pivotCache cacheId="13" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="124">
   <si>
     <t>Date</t>
   </si>
@@ -152,9 +152,6 @@
   </si>
   <si>
     <t>AMICI PIZZA</t>
-  </si>
-  <si>
-    <t>Jeff Pay</t>
   </si>
   <si>
     <t>COLUMBUS CITY TREASURY</t>
@@ -516,6 +513,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -524,7 +522,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1670,7 +1667,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1870C13B-AC88-4747-AFC0-996355F07F2B}" name="PivotTable3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1870C13B-AC88-4747-AFC0-996355F07F2B}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -1789,18 +1786,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}" name="Table1" displayName="Table1" ref="A1:F125" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}" name="Table1" displayName="Table1" ref="A1:F125" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F125" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F125">
     <sortCondition ref="A1:A125"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{36D6B367-4586-164A-BAFD-F61BD8D7B0D8}" name="Date" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{163A618F-4E2A-CF42-8DEE-891E741B2D57}" name="Source" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{49FF6B6D-B6DF-3C46-990B-4A21BE1D1B1E}" name="Transaction" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{84AF5D09-AAE0-8848-B5A8-C38A5769933E}" name="Category" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{0A1EF426-6D1D-AF40-9C65-9FAE6E780C77}" name="Amount" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{BA3274DD-10C7-F14A-8D5D-C0FF14C09BB2}" name="Type" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{36D6B367-4586-164A-BAFD-F61BD8D7B0D8}" name="Date" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{163A618F-4E2A-CF42-8DEE-891E741B2D57}" name="Source" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{49FF6B6D-B6DF-3C46-990B-4A21BE1D1B1E}" name="Transaction" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{84AF5D09-AAE0-8848-B5A8-C38A5769933E}" name="Category" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{0A1EF426-6D1D-AF40-9C65-9FAE6E780C77}" name="Amount" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{BA3274DD-10C7-F14A-8D5D-C0FF14C09BB2}" name="Type" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2106,7 +2103,7 @@
   <dimension ref="A1:F125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2134,7 +2131,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2148,13 +2145,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="6">
-        <v>-300</v>
+        <v>-50</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2162,19 +2159,19 @@
         <v>44774</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E3" s="6">
-        <v>-50</v>
+        <v>-12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2182,19 +2179,19 @@
         <v>44774</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E4" s="6">
-        <v>-12</v>
+        <v>-300</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2215,7 +2212,7 @@
         <v>300</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2226,16 +2223,16 @@
         <v>23</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6">
-        <v>-847.99</v>
+        <v>-5.93</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2243,20 +2240,19 @@
         <v>44776</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" s="6">
-        <f>-85.23-E6</f>
-        <v>762.76</v>
+        <v>-36</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2264,19 +2260,19 @@
         <v>44776</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="6">
-        <v>-36</v>
+        <v>-26.34</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2284,19 +2280,19 @@
         <v>44776</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E9" s="6">
-        <v>-35.880000000000003</v>
+        <v>-847.99</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2307,16 +2303,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E10" s="6">
-        <v>-26.34</v>
+        <v>-35.880000000000003</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2336,7 +2332,7 @@
         <v>-24</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2344,16 +2340,17 @@
         <v>44776</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="E12" s="6">
-        <v>-5.93</v>
+        <f>--3.19</f>
+        <v>3.19</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>121</v>
@@ -2370,14 +2367,14 @@
         <v>25</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E13" s="6">
-        <f>--3.19</f>
-        <v>3.19</v>
+        <f>-85.23-E12</f>
+        <v>-88.42</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2385,19 +2382,19 @@
         <v>44778</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E14" s="6">
-        <v>-117</v>
+        <v>-22.5</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2408,13 +2405,14 @@
         <v>7</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" s="6">
-        <v>-22.5</v>
+        <f>--2.5</f>
+        <v>2.5</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>121</v>
@@ -2428,16 +2426,16 @@
         <v>23</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E16" s="6">
-        <v>-9.5299999999999994</v>
+        <v>-117</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -2454,10 +2452,10 @@
         <v>12</v>
       </c>
       <c r="E17" s="6">
-        <v>-7.21</v>
+        <v>-9.5299999999999994</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2465,20 +2463,19 @@
         <v>44778</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E18" s="6">
-        <f>--2.5</f>
-        <v>2.5</v>
+        <v>-7.21</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -2489,16 +2486,16 @@
         <v>23</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="6">
-        <v>-47.94</v>
+        <v>-19.71</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2509,16 +2506,16 @@
         <v>23</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E20" s="6">
-        <v>-19.71</v>
+        <v>-47.94</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2529,16 +2526,16 @@
         <v>23</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="6">
         <v>-97.9</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2546,19 +2543,19 @@
         <v>44782</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E22" s="6">
-        <v>-121.08</v>
+        <v>-2.99</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2572,13 +2569,13 @@
         <v>25</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E23" s="6">
-        <v>-50.35</v>
+        <v>-42.99</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -2586,19 +2583,19 @@
         <v>44782</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="E24" s="6">
-        <v>-42.99</v>
+        <v>-32</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -2606,19 +2603,20 @@
         <v>44782</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="6">
-        <v>-32</v>
+        <f>-5.49-1.19</f>
+        <v>-6.68</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -2635,10 +2633,10 @@
         <v>43</v>
       </c>
       <c r="E26" s="6">
-        <v>-18.690000000000001</v>
+        <v>-50.35</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -2652,14 +2650,13 @@
         <v>25</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E27" s="6">
-        <f>-5.49-1.19</f>
-        <v>-6.68</v>
+        <v>-6.33</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -2676,10 +2673,10 @@
         <v>11</v>
       </c>
       <c r="E28" s="6">
-        <v>-6.33</v>
+        <v>-5.12</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2693,13 +2690,13 @@
         <v>25</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="E29" s="6">
-        <v>-5.12</v>
+        <v>-18.690000000000001</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2707,19 +2704,19 @@
         <v>44782</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="E30" s="6">
-        <v>-2.99</v>
+        <v>-121.08</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -2730,17 +2727,17 @@
         <v>7</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E31" s="6">
         <f>--4428.13</f>
         <v>4428.13</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -2751,7 +2748,7 @@
         <v>23</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>12</v>
@@ -2760,7 +2757,7 @@
         <v>-195.11</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -2771,7 +2768,7 @@
         <v>23</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>11</v>
@@ -2780,7 +2777,7 @@
         <v>-13.36</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -2791,16 +2788,16 @@
         <v>23</v>
       </c>
       <c r="C34" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="E34" s="6">
         <v>-103.59</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2811,16 +2808,16 @@
         <v>23</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E35" s="6">
         <v>-82.78</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -2828,16 +2825,17 @@
         <v>44785</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E36" s="6">
-        <v>-29.47</v>
+        <f>--2856.77</f>
+        <v>2856.77</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>121</v>
@@ -2848,20 +2846,19 @@
         <v>44785</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E37" s="6">
-        <f>--2856.77</f>
-        <v>2856.77</v>
+        <v>-29.47</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -2872,7 +2869,7 @@
         <v>23</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>31</v>
@@ -2881,7 +2878,7 @@
         <v>-9.5299999999999994</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -2895,13 +2892,13 @@
         <v>28</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E39" s="6">
-        <v>-134.43</v>
+        <v>-37.78</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -2912,16 +2909,16 @@
         <v>23</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="E40" s="6">
-        <v>-82.58</v>
+        <v>-134.43</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2932,16 +2929,16 @@
         <v>23</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E41" s="6">
-        <v>-37.78</v>
+        <v>-82.58</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2955,13 +2952,13 @@
         <v>28</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E42" s="6">
         <v>-10.99</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2972,16 +2969,16 @@
         <v>7</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="E43" s="6">
-        <v>-4500</v>
+        <v>-1935.13</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2989,16 +2986,17 @@
         <v>44788</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E44" s="6">
-        <v>-1935.13</v>
+        <f>--1935.13</f>
+        <v>1935.13</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>121</v>
@@ -3015,13 +3013,13 @@
         <v>6</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E45" s="6">
-        <v>-300</v>
+        <v>-50</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -3032,16 +3030,16 @@
         <v>7</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E46" s="6">
-        <v>-50</v>
+        <v>-16.55</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -3049,19 +3047,19 @@
         <v>44788</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E47" s="6">
-        <v>-24</v>
+        <v>-9.99</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -3069,19 +3067,19 @@
         <v>44788</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E48" s="6">
-        <v>-16.55</v>
+        <v>-24</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -3089,16 +3087,17 @@
         <v>44788</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E49" s="6">
-        <v>-9.99</v>
+        <f>--413</f>
+        <v>413</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>121</v>
@@ -3109,20 +3108,19 @@
         <v>44788</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E50" s="6">
-        <f>--300</f>
-        <v>300</v>
+        <v>-4500</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -3130,20 +3128,19 @@
         <v>44788</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="E51" s="6">
-        <f>--413</f>
-        <v>413</v>
+        <v>-300</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -3151,20 +3148,20 @@
         <v>44788</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="E52" s="6">
-        <f>--1935.13</f>
-        <v>1935.13</v>
+        <f>--300</f>
+        <v>300</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -3185,7 +3182,7 @@
         <v>4500</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -3193,19 +3190,19 @@
         <v>44789</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="E54" s="6">
-        <v>-12000</v>
+        <v>-60.05</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -3213,19 +3210,19 @@
         <v>44789</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E55" s="6">
-        <v>-60.05</v>
+        <v>-12000</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -3233,16 +3230,17 @@
         <v>44791</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="E56" s="6">
-        <v>-23.1</v>
+        <f>--0.04</f>
+        <v>0.04</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>121</v>
@@ -3256,16 +3254,16 @@
         <v>23</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E57" s="6">
         <v>-15.98</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -3273,20 +3271,19 @@
         <v>44791</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="E58" s="6">
-        <f>--0.04</f>
-        <v>0.04</v>
+        <v>-23.1</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -3294,19 +3291,19 @@
         <v>44792</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E59" s="6">
-        <v>-57.39</v>
+        <v>-17.78</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -3320,13 +3317,13 @@
         <v>25</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="E60" s="6">
-        <v>-52.46</v>
+        <v>-14.08</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -3340,13 +3337,13 @@
         <v>25</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="E61" s="6">
-        <v>-19.87</v>
+        <v>-6</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -3360,13 +3357,13 @@
         <v>25</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="E62" s="6">
-        <v>-17.78</v>
+        <v>-19.87</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -3380,13 +3377,13 @@
         <v>25</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E63" s="6">
-        <v>-14.08</v>
+        <v>-6</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -3394,19 +3391,19 @@
         <v>44792</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E64" s="6">
-        <v>-13.95</v>
+        <v>-57.39</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -3420,13 +3417,13 @@
         <v>25</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E65" s="6">
-        <v>-6</v>
+        <v>-52.46</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -3440,13 +3437,13 @@
         <v>25</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E66" s="6">
-        <v>-6</v>
+        <v>-13.95</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -3457,16 +3454,16 @@
         <v>23</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E67" s="6">
         <v>-39.99</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -3477,16 +3474,16 @@
         <v>7</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E68" s="6">
         <v>-883.65</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -3497,16 +3494,16 @@
         <v>23</v>
       </c>
       <c r="C69" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D69" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="E69" s="6">
         <v>-145.75</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -3517,16 +3514,16 @@
         <v>23</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E70" s="6">
         <v>-65.05</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -3537,16 +3534,16 @@
         <v>23</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E71" s="6">
-        <v>-24.5</v>
+        <v>-14.11</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -3560,13 +3557,13 @@
         <v>90</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E72" s="6">
-        <v>-14.11</v>
+        <v>-24.5</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -3577,7 +3574,7 @@
         <v>23</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>11</v>
@@ -3586,7 +3583,7 @@
         <v>-10</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -3600,10 +3597,11 @@
         <v>25</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E74" s="6">
-        <v>-53.71</v>
+        <f>--33.08</f>
+        <v>33.08</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>121</v>
@@ -3620,13 +3618,13 @@
         <v>25</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="E75" s="6">
-        <v>-34.79</v>
+        <v>-28.47</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -3640,13 +3638,13 @@
         <v>25</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E76" s="6">
-        <v>-28.47</v>
+        <v>-34.79</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -3654,19 +3652,19 @@
         <v>44797</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E77" s="6">
-        <v>-24.21</v>
+        <v>-7.48</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -3680,13 +3678,13 @@
         <v>25</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="E78" s="6">
-        <v>-12.99</v>
+        <v>-53.71</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -3700,10 +3698,11 @@
         <v>25</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E79" s="6">
-        <v>-7.48</v>
+        <f>--3.7</f>
+        <v>3.7</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>121</v>
@@ -3714,16 +3713,17 @@
         <v>44797</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E80" s="6">
-        <v>-4.7</v>
+        <f>--5.71</f>
+        <v>5.71</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>121</v>
@@ -3740,14 +3740,13 @@
         <v>25</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="E81" s="6">
-        <f>--3.7</f>
-        <v>3.7</v>
+        <v>-12.99</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -3755,20 +3754,19 @@
         <v>44797</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E82" s="6">
-        <f>--5.71</f>
-        <v>5.71</v>
+        <v>-24.21</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -3776,20 +3774,19 @@
         <v>44797</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="E83" s="6">
-        <f>--33.08</f>
-        <v>33.08</v>
+        <v>-4.7</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -3800,16 +3797,16 @@
         <v>7</v>
       </c>
       <c r="C84" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D84" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="E84" s="6">
         <v>-300</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -3820,7 +3817,7 @@
         <v>23</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>12</v>
@@ -3829,7 +3826,7 @@
         <v>-32.270000000000003</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -3840,7 +3837,7 @@
         <v>23</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>31</v>
@@ -3849,7 +3846,7 @@
         <v>-19.34</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -3860,16 +3857,16 @@
         <v>23</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E87" s="6">
         <v>-57.09</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -3880,16 +3877,16 @@
         <v>23</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E88" s="6">
         <v>-30.95</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -3900,7 +3897,7 @@
         <v>23</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>12</v>
@@ -3909,7 +3906,7 @@
         <v>-17.36</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -3920,7 +3917,7 @@
         <v>23</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>31</v>
@@ -3929,7 +3926,7 @@
         <v>-6.77</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -3940,16 +3937,16 @@
         <v>23</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E91" s="6">
         <v>-26.67</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -3960,7 +3957,7 @@
         <v>23</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>31</v>
@@ -3969,7 +3966,7 @@
         <v>-18.64</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -3983,13 +3980,13 @@
         <v>109</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E93" s="6">
-        <v>-43.6</v>
+        <v>-15.04</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -4003,13 +4000,13 @@
         <v>111</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E94" s="6">
-        <v>-34.11</v>
+        <v>-25</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -4020,16 +4017,16 @@
         <v>23</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E95" s="6">
-        <v>-25</v>
+        <v>-43.6</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -4043,13 +4040,13 @@
         <v>110</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E96" s="6">
-        <v>-15.04</v>
+        <v>-34.11</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -4060,16 +4057,16 @@
         <v>7</v>
       </c>
       <c r="C97" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D97" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D97" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="E97" s="6">
-        <v>-965.06</v>
+        <v>-38</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -4080,16 +4077,16 @@
         <v>7</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="E98" s="6">
-        <v>-63.5</v>
+        <v>-965.06</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -4097,16 +4094,17 @@
         <v>44802</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E99" s="6">
-        <v>-38</v>
+        <f>--965.06</f>
+        <v>965.06</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>121</v>
@@ -4117,16 +4115,16 @@
         <v>44802</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E100" s="6">
-        <v>-24</v>
+        <v>13.99</v>
       </c>
       <c r="F100" s="6" t="s">
         <v>121</v>
@@ -4137,16 +4135,16 @@
         <v>44802</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="E101" s="6">
-        <v>-9.99</v>
+        <v>12.99</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>121</v>
@@ -4157,19 +4155,19 @@
         <v>44802</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>114</v>
+        <v>12</v>
       </c>
       <c r="E102" s="6">
-        <v>-9.44</v>
+        <v>-2.29</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -4177,19 +4175,19 @@
         <v>44802</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E103" s="6">
-        <v>-2.29</v>
+        <v>-24</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -4197,19 +4195,19 @@
         <v>44802</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>25</v>
+        <v>107</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="E104" s="6">
-        <v>12.99</v>
+        <v>-9.99</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -4223,13 +4221,13 @@
         <v>25</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E105" s="6">
-        <v>13.99</v>
+        <v>-63.5</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -4240,17 +4238,16 @@
         <v>23</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>63</v>
+        <v>113</v>
       </c>
       <c r="E106" s="6">
-        <f>--965.06</f>
-        <v>965.06</v>
+        <v>-9.44</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -4261,16 +4258,16 @@
         <v>7</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E107" s="6">
         <v>-335.43</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -4281,16 +4278,16 @@
         <v>23</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E108" s="6">
         <v>-210</v>
       </c>
       <c r="F108" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -4301,7 +4298,7 @@
         <v>23</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>32</v>
@@ -4310,7 +4307,7 @@
         <v>-24</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -4321,16 +4318,16 @@
         <v>23</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E110" s="6">
         <v>-13</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -4338,16 +4335,17 @@
         <v>44804</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E111" s="6">
-        <v>-50.52</v>
+        <f>--0.12</f>
+        <v>0.12</v>
       </c>
       <c r="F111" s="6" t="s">
         <v>121</v>
@@ -4358,20 +4356,19 @@
         <v>44804</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E112" s="6">
-        <f>--0.12</f>
-        <v>0.12</v>
+        <v>-50.52</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -4382,17 +4379,17 @@
         <v>7</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>41</v>
       </c>
       <c r="E113" s="6">
-        <f>--614.79</f>
-        <v>614.79</v>
+        <f>--3116.22</f>
+        <v>3116.22</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -4406,14 +4403,14 @@
         <v>95</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E114" s="6">
-        <f>--3116.22</f>
-        <v>3116.22</v>
+        <f>--614.79</f>
+        <v>614.79</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -4427,13 +4424,13 @@
         <v>6</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E115" s="6">
-        <v>-3000</v>
+        <v>-50</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -4450,10 +4447,10 @@
         <v>9</v>
       </c>
       <c r="E116" s="6">
-        <v>-300</v>
+        <v>-3000</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -4467,13 +4464,13 @@
         <v>6</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E117" s="6">
-        <v>-50</v>
+        <v>-300</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -4494,7 +4491,7 @@
         <v>300</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -4515,7 +4512,7 @@
         <v>3000</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -4526,16 +4523,16 @@
         <v>23</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E120" s="6">
         <v>-25</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -4546,16 +4543,16 @@
         <v>23</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E121" s="6">
         <v>-18</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -4569,13 +4566,13 @@
         <v>97</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="E122" s="6">
-        <v>-13.41</v>
+        <v>-10</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -4586,16 +4583,16 @@
         <v>23</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E123" s="6">
-        <v>-10</v>
+        <v>-6</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -4606,16 +4603,16 @@
         <v>23</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E124" s="6">
-        <v>-8.9</v>
+        <v>-13.41</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -4626,16 +4623,16 @@
         <v>23</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="E125" s="6">
-        <v>-6</v>
+        <v>-8.9</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4683,7 +4680,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
@@ -4693,37 +4690,37 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
@@ -4733,7 +4730,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
@@ -4743,7 +4740,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
@@ -4758,17 +4755,17 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
@@ -4783,17 +4780,17 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
@@ -4808,17 +4805,17 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
@@ -4838,7 +4835,7 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -4875,34 +4872,34 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" t="s">
         <v>115</v>
-      </c>
-      <c r="C4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="2">
         <v>19504.420000000002</v>
@@ -4916,7 +4913,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" s="2">
         <v>3300</v>
@@ -4930,7 +4927,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="2">
         <v>22804.420000000002</v>

</xml_diff>

<commit_message>
Updated a few expense categories
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffgood/Desktop/R_Studio_Projects/Financial_Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35595B41-A7EA-E54C-AA53-CD96E62AA944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74306D5C-CDC4-794B-A716-A69C872866E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="1000" windowWidth="27380" windowHeight="15800" xr2:uid="{D9F47917-7B20-384C-878F-0D08681ABD47}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId4"/>
+    <pivotCache cacheId="15" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="125">
   <si>
     <t>Date</t>
   </si>
@@ -232,9 +232,6 @@
     <t>Books</t>
   </si>
   <si>
-    <t>Credit_Card_Payment</t>
-  </si>
-  <si>
     <t>VANGUARD BUY     INVESTMENT ***********3619</t>
   </si>
   <si>
@@ -416,6 +413,12 @@
   </si>
   <si>
     <t>(All)</t>
+  </si>
+  <si>
+    <t>USAA_CC_Payment</t>
+  </si>
+  <si>
+    <t>Chase_CC_Payment</t>
   </si>
 </sst>
 </file>
@@ -1667,7 +1670,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1870C13B-AC88-4747-AFC0-996355F07F2B}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1870C13B-AC88-4747-AFC0-996355F07F2B}" name="PivotTable3" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -2103,7 +2106,7 @@
   <dimension ref="A1:F125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2131,7 +2134,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2151,7 +2154,7 @@
         <v>-50</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2171,7 +2174,7 @@
         <v>-12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2191,7 +2194,7 @@
         <v>-300</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2212,7 +2215,7 @@
         <v>300</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2232,7 +2235,7 @@
         <v>-5.93</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2252,7 +2255,7 @@
         <v>-36</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2272,7 +2275,7 @@
         <v>-26.34</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2292,7 +2295,7 @@
         <v>-847.99</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2312,7 +2315,7 @@
         <v>-35.880000000000003</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2332,7 +2335,7 @@
         <v>-24</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2353,7 +2356,7 @@
         <v>3.19</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2374,7 +2377,7 @@
         <v>-88.42</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2394,7 +2397,7 @@
         <v>-22.5</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2415,7 +2418,7 @@
         <v>2.5</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2435,7 +2438,7 @@
         <v>-117</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -2455,7 +2458,7 @@
         <v>-9.5299999999999994</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2475,7 +2478,7 @@
         <v>-7.21</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -2495,7 +2498,7 @@
         <v>-19.71</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2515,7 +2518,7 @@
         <v>-47.94</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2535,7 +2538,7 @@
         <v>-97.9</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2555,7 +2558,7 @@
         <v>-2.99</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2575,7 +2578,7 @@
         <v>-42.99</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -2595,7 +2598,7 @@
         <v>-32</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -2616,7 +2619,7 @@
         <v>-6.68</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -2636,7 +2639,7 @@
         <v>-50.35</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -2656,7 +2659,7 @@
         <v>-6.33</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -2676,7 +2679,7 @@
         <v>-5.12</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2696,7 +2699,7 @@
         <v>-18.690000000000001</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2716,7 +2719,7 @@
         <v>-121.08</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -2737,7 +2740,7 @@
         <v>4428.13</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -2757,7 +2760,7 @@
         <v>-195.11</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -2777,7 +2780,7 @@
         <v>-13.36</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -2797,7 +2800,7 @@
         <v>-103.59</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2817,7 +2820,7 @@
         <v>-82.78</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -2838,7 +2841,7 @@
         <v>2856.77</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -2858,7 +2861,7 @@
         <v>-29.47</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -2878,7 +2881,7 @@
         <v>-9.5299999999999994</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -2898,7 +2901,7 @@
         <v>-37.78</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -2918,7 +2921,7 @@
         <v>-134.43</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2929,7 +2932,7 @@
         <v>23</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>56</v>
@@ -2938,7 +2941,7 @@
         <v>-82.58</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2958,7 +2961,7 @@
         <v>-10.99</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2972,13 +2975,13 @@
         <v>58</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="E43" s="6">
         <v>-1935.13</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2989,17 +2992,17 @@
         <v>23</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="E44" s="6">
         <f>--1935.13</f>
         <v>1935.13</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -3019,7 +3022,7 @@
         <v>-50</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -3039,7 +3042,7 @@
         <v>-16.55</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -3059,7 +3062,7 @@
         <v>-9.99</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -3070,7 +3073,7 @@
         <v>23</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>32</v>
@@ -3079,7 +3082,7 @@
         <v>-24</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -3090,7 +3093,7 @@
         <v>18</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>40</v>
@@ -3100,7 +3103,7 @@
         <v>413</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -3120,7 +3123,7 @@
         <v>-4500</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -3140,7 +3143,7 @@
         <v>-300</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -3161,7 +3164,7 @@
         <v>300</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -3182,7 +3185,7 @@
         <v>4500</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -3193,7 +3196,7 @@
         <v>23</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>12</v>
@@ -3202,7 +3205,7 @@
         <v>-60.05</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -3213,16 +3216,16 @@
         <v>18</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E55" s="6">
         <v>-12000</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -3243,7 +3246,7 @@
         <v>0.04</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -3254,7 +3257,7 @@
         <v>23</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>61</v>
@@ -3263,7 +3266,7 @@
         <v>-15.98</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -3274,16 +3277,16 @@
         <v>23</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E58" s="6">
         <v>-23.1</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -3303,7 +3306,7 @@
         <v>-17.78</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -3323,7 +3326,7 @@
         <v>-14.08</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -3343,7 +3346,7 @@
         <v>-6</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -3363,7 +3366,7 @@
         <v>-19.87</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -3383,7 +3386,7 @@
         <v>-6</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -3394,7 +3397,7 @@
         <v>23</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>56</v>
@@ -3403,7 +3406,7 @@
         <v>-57.39</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -3423,7 +3426,7 @@
         <v>-52.46</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -3443,7 +3446,7 @@
         <v>-13.95</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -3454,16 +3457,16 @@
         <v>23</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E67" s="6">
         <v>-39.99</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -3474,16 +3477,16 @@
         <v>7</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="E68" s="6">
         <v>-883.65</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -3494,16 +3497,16 @@
         <v>23</v>
       </c>
       <c r="C69" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D69" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="E69" s="6">
         <v>-145.75</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -3514,7 +3517,7 @@
         <v>23</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>44</v>
@@ -3523,7 +3526,7 @@
         <v>-65.05</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -3534,7 +3537,7 @@
         <v>23</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>12</v>
@@ -3543,7 +3546,7 @@
         <v>-14.11</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -3554,7 +3557,7 @@
         <v>23</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>32</v>
@@ -3563,7 +3566,7 @@
         <v>-24.5</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -3574,7 +3577,7 @@
         <v>23</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>11</v>
@@ -3583,7 +3586,7 @@
         <v>-10</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -3604,7 +3607,7 @@
         <v>33.08</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -3618,13 +3621,13 @@
         <v>25</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E75" s="6">
         <v>-28.47</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -3644,7 +3647,7 @@
         <v>-34.79</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -3664,7 +3667,7 @@
         <v>-7.48</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -3678,13 +3681,13 @@
         <v>25</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E78" s="6">
         <v>-53.71</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -3705,7 +3708,7 @@
         <v>3.7</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -3726,7 +3729,7 @@
         <v>5.71</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -3746,7 +3749,7 @@
         <v>-12.99</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -3757,7 +3760,7 @@
         <v>23</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>31</v>
@@ -3766,7 +3769,7 @@
         <v>-24.21</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -3777,7 +3780,7 @@
         <v>23</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>31</v>
@@ -3786,7 +3789,7 @@
         <v>-4.7</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -3797,16 +3800,16 @@
         <v>7</v>
       </c>
       <c r="C84" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D84" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="E84" s="6">
         <v>-300</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -3817,7 +3820,7 @@
         <v>23</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>12</v>
@@ -3826,7 +3829,7 @@
         <v>-32.270000000000003</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -3837,7 +3840,7 @@
         <v>23</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>31</v>
@@ -3846,7 +3849,7 @@
         <v>-19.34</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -3857,7 +3860,7 @@
         <v>23</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>44</v>
@@ -3866,7 +3869,7 @@
         <v>-57.09</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -3877,7 +3880,7 @@
         <v>23</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>44</v>
@@ -3886,7 +3889,7 @@
         <v>-30.95</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -3897,7 +3900,7 @@
         <v>23</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>12</v>
@@ -3906,7 +3909,7 @@
         <v>-17.36</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -3917,7 +3920,7 @@
         <v>23</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>31</v>
@@ -3926,7 +3929,7 @@
         <v>-6.77</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -3937,7 +3940,7 @@
         <v>23</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>59</v>
@@ -3946,7 +3949,7 @@
         <v>-26.67</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -3957,7 +3960,7 @@
         <v>23</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>31</v>
@@ -3966,7 +3969,7 @@
         <v>-18.64</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -3977,7 +3980,7 @@
         <v>23</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>30</v>
@@ -3986,7 +3989,7 @@
         <v>-15.04</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -3997,7 +4000,7 @@
         <v>23</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>11</v>
@@ -4006,7 +4009,7 @@
         <v>-25</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -4017,7 +4020,7 @@
         <v>23</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>31</v>
@@ -4026,7 +4029,7 @@
         <v>-43.6</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -4037,7 +4040,7 @@
         <v>23</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>31</v>
@@ -4046,7 +4049,7 @@
         <v>-34.11</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -4066,7 +4069,7 @@
         <v>-38</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -4080,13 +4083,13 @@
         <v>58</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="E98" s="6">
         <v>-965.06</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -4097,17 +4100,17 @@
         <v>23</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="E99" s="6">
         <f>--965.06</f>
         <v>965.06</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -4127,7 +4130,7 @@
         <v>13.99</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -4141,13 +4144,13 @@
         <v>25</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E101" s="6">
         <v>12.99</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -4167,7 +4170,7 @@
         <v>-2.29</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -4178,7 +4181,7 @@
         <v>23</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>32</v>
@@ -4187,7 +4190,7 @@
         <v>-24</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -4198,7 +4201,7 @@
         <v>23</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>11</v>
@@ -4207,7 +4210,7 @@
         <v>-9.99</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -4227,7 +4230,7 @@
         <v>-63.5</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -4238,16 +4241,16 @@
         <v>23</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E106" s="6">
         <v>-9.44</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -4258,16 +4261,16 @@
         <v>7</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="E107" s="6">
         <v>-335.43</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -4278,16 +4281,16 @@
         <v>23</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E108" s="6">
         <v>-210</v>
       </c>
       <c r="F108" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -4298,7 +4301,7 @@
         <v>23</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>32</v>
@@ -4307,7 +4310,7 @@
         <v>-24</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -4318,7 +4321,7 @@
         <v>23</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>42</v>
@@ -4327,7 +4330,7 @@
         <v>-13</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -4348,7 +4351,7 @@
         <v>0.12</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -4359,7 +4362,7 @@
         <v>23</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>12</v>
@@ -4368,7 +4371,7 @@
         <v>-50.52</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -4379,7 +4382,7 @@
         <v>7</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>41</v>
@@ -4389,7 +4392,7 @@
         <v>3116.22</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -4400,7 +4403,7 @@
         <v>7</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>40</v>
@@ -4410,7 +4413,7 @@
         <v>614.79</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -4430,7 +4433,7 @@
         <v>-50</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -4450,7 +4453,7 @@
         <v>-3000</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -4470,7 +4473,7 @@
         <v>-300</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -4491,7 +4494,7 @@
         <v>300</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -4512,7 +4515,7 @@
         <v>3000</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -4523,16 +4526,16 @@
         <v>23</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E120" s="6">
         <v>-25</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -4543,16 +4546,16 @@
         <v>23</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E121" s="6">
         <v>-18</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -4563,16 +4566,16 @@
         <v>23</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E122" s="6">
         <v>-10</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -4583,16 +4586,16 @@
         <v>23</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E123" s="6">
         <v>-6</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -4603,7 +4606,7 @@
         <v>23</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>31</v>
@@ -4612,7 +4615,7 @@
         <v>-13.41</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -4623,7 +4626,7 @@
         <v>23</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>31</v>
@@ -4632,7 +4635,7 @@
         <v>-8.9</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -4657,10 +4660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A85DC7-AAE6-0D45-BE57-A2D20F484BD4}">
-  <dimension ref="A1:A34"/>
+  <dimension ref="A1:A35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4695,27 +4698,27 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
@@ -4730,7 +4733,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
@@ -4755,7 +4758,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
@@ -4780,12 +4783,12 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
@@ -4815,7 +4818,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
@@ -4835,13 +4838,18 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:A9" xr:uid="{92A85DC7-AAE6-0D45-BE57-A2D20F484BD4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A34">
-      <sortCondition ref="A1:A34"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A35">
+      <sortCondition ref="A1:A35"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4872,34 +4880,34 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" t="s">
         <v>114</v>
-      </c>
-      <c r="C4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E4" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="2">
         <v>19504.420000000002</v>
@@ -4913,7 +4921,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="2">
         <v>3300</v>
@@ -4927,7 +4935,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="2">
         <v>22804.420000000002</v>

</xml_diff>

<commit_message>
weekly expenses update update syntax
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffgood/Desktop/R_Studio_Projects/Financial_Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0C158D-598D-644A-B210-5D038AF14E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAFDB17-3D60-0145-8060-6AA11DFAAC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1000" windowWidth="15380" windowHeight="15800" xr2:uid="{D9F47917-7B20-384C-878F-0D08681ABD47}"/>
+    <workbookView xWindow="20" yWindow="1000" windowWidth="15420" windowHeight="15800" xr2:uid="{D9F47917-7B20-384C-878F-0D08681ABD47}"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="256">
   <si>
     <t>Date</t>
   </si>
@@ -788,6 +788,30 @@
   </si>
   <si>
     <t>Reebok</t>
+  </si>
+  <si>
+    <t>Federal Payment</t>
+  </si>
+  <si>
+    <t>IN *D &amp; M HANES INC.     419-4255550  OH</t>
+  </si>
+  <si>
+    <t>Chipotle</t>
+  </si>
+  <si>
+    <t>Etsy</t>
+  </si>
+  <si>
+    <t>Performasleep</t>
+  </si>
+  <si>
+    <t>Informs.org</t>
+  </si>
+  <si>
+    <t>Ohio Military</t>
+  </si>
+  <si>
+    <t>Lowe's</t>
   </si>
 </sst>
 </file>
@@ -2157,10 +2181,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}" name="Table1" displayName="Table1" ref="A1:E384" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E384" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E384">
-    <sortCondition ref="A1:A384"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}" name="Table1" displayName="Table1" ref="A1:E415" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E415" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E415">
+    <sortCondition ref="A1:A415"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{36D6B367-4586-164A-BAFD-F61BD8D7B0D8}" name="Date" dataDxfId="4"/>
@@ -2470,10 +2494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BEBEFE-BF8C-CE41-8907-E9633ACA1DDB}">
-  <dimension ref="A1:E384"/>
+  <dimension ref="A1:E415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A370" workbookViewId="0">
-      <selection activeCell="D374" sqref="D374"/>
+    <sheetView tabSelected="1" topLeftCell="A408" workbookViewId="0">
+      <selection activeCell="D408" sqref="D408"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9049,6 +9073,533 @@
         <v>300</v>
       </c>
     </row>
+    <row r="385" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A385" s="5">
+        <v>44880</v>
+      </c>
+      <c r="B385" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C385" t="s">
+        <v>255</v>
+      </c>
+      <c r="D385" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E385">
+        <v>-80.33</v>
+      </c>
+    </row>
+    <row r="386" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A386" s="5">
+        <v>44880</v>
+      </c>
+      <c r="B386" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C386" t="s">
+        <v>73</v>
+      </c>
+      <c r="D386" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E386">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A387" s="5">
+        <v>44880</v>
+      </c>
+      <c r="B387" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C387" t="s">
+        <v>198</v>
+      </c>
+      <c r="D387" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E387">
+        <v>-19.7</v>
+      </c>
+    </row>
+    <row r="388" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A388" s="5">
+        <v>44881</v>
+      </c>
+      <c r="B388" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C388" t="s">
+        <v>202</v>
+      </c>
+      <c r="D388" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E388">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="389" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A389" s="5">
+        <v>44881</v>
+      </c>
+      <c r="B389" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C389" t="s">
+        <v>248</v>
+      </c>
+      <c r="D389" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E389">
+        <v>347.5</v>
+      </c>
+    </row>
+    <row r="390" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A390" s="5">
+        <v>44881</v>
+      </c>
+      <c r="B390" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C390" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D390" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E390" s="6">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="391" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A391" s="5">
+        <v>44881</v>
+      </c>
+      <c r="B391" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C391" t="s">
+        <v>254</v>
+      </c>
+      <c r="D391" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E391">
+        <v>-26.25</v>
+      </c>
+    </row>
+    <row r="392" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A392" s="5">
+        <v>44881</v>
+      </c>
+      <c r="B392" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C392" t="s">
+        <v>187</v>
+      </c>
+      <c r="D392" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E392">
+        <v>376.29</v>
+      </c>
+    </row>
+    <row r="393" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A393" s="5">
+        <v>44882</v>
+      </c>
+      <c r="B393" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C393" t="s">
+        <v>253</v>
+      </c>
+      <c r="D393" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E393">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="394" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A394" s="5">
+        <v>44884</v>
+      </c>
+      <c r="B394" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C394" t="s">
+        <v>207</v>
+      </c>
+      <c r="D394" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E394">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="395" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A395" s="5">
+        <v>44884</v>
+      </c>
+      <c r="B395" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C395" t="s">
+        <v>185</v>
+      </c>
+      <c r="D395" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E395">
+        <v>-75.48</v>
+      </c>
+    </row>
+    <row r="396" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A396" s="5">
+        <v>44884</v>
+      </c>
+      <c r="B396" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C396" t="s">
+        <v>185</v>
+      </c>
+      <c r="D396" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E396" s="6">
+        <v>-134.57</v>
+      </c>
+    </row>
+    <row r="397" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A397" s="5">
+        <v>44884</v>
+      </c>
+      <c r="B397" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C397" t="s">
+        <v>185</v>
+      </c>
+      <c r="D397" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E397" s="6">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="398" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A398" s="5">
+        <v>44884</v>
+      </c>
+      <c r="B398" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C398" t="s">
+        <v>185</v>
+      </c>
+      <c r="D398" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E398" s="6">
+        <v>-82.96</v>
+      </c>
+    </row>
+    <row r="399" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A399" s="5">
+        <v>44884</v>
+      </c>
+      <c r="B399" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C399" t="s">
+        <v>185</v>
+      </c>
+      <c r="D399" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E399" s="6">
+        <v>-53.98</v>
+      </c>
+    </row>
+    <row r="400" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A400" s="5">
+        <v>44884</v>
+      </c>
+      <c r="B400" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C400" t="s">
+        <v>185</v>
+      </c>
+      <c r="D400" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E400" s="6">
+        <v>-18.989999999999998</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A401" s="5">
+        <v>44884</v>
+      </c>
+      <c r="B401" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C401" t="s">
+        <v>185</v>
+      </c>
+      <c r="D401" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E401" s="6">
+        <v>-48.07</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A402" s="5">
+        <v>44884</v>
+      </c>
+      <c r="B402" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C402" t="s">
+        <v>185</v>
+      </c>
+      <c r="D402" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E402" s="6">
+        <v>-9.99</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A403" s="5">
+        <v>44884</v>
+      </c>
+      <c r="B403" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C403" t="s">
+        <v>251</v>
+      </c>
+      <c r="D403" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E403">
+        <v>-87.21</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A404" s="5">
+        <v>44884</v>
+      </c>
+      <c r="B404" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C404" t="s">
+        <v>252</v>
+      </c>
+      <c r="D404" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E404">
+        <v>-79.5</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A405" s="5">
+        <v>44885</v>
+      </c>
+      <c r="B405" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C405" t="s">
+        <v>249</v>
+      </c>
+      <c r="D405" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E405">
+        <v>-35</v>
+      </c>
+    </row>
+    <row r="406" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A406" s="5">
+        <v>44885</v>
+      </c>
+      <c r="B406" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C406" t="s">
+        <v>129</v>
+      </c>
+      <c r="D406" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E406">
+        <v>-184.05</v>
+      </c>
+    </row>
+    <row r="407" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A407" s="5">
+        <v>44885</v>
+      </c>
+      <c r="B407" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C407" t="s">
+        <v>127</v>
+      </c>
+      <c r="D407" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E407">
+        <v>-27.45</v>
+      </c>
+    </row>
+    <row r="408" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A408" s="5">
+        <v>44885</v>
+      </c>
+      <c r="B408" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C408" t="s">
+        <v>127</v>
+      </c>
+      <c r="D408" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E408">
+        <v>-61.99</v>
+      </c>
+    </row>
+    <row r="409" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A409" s="5">
+        <v>44885</v>
+      </c>
+      <c r="B409" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C409" t="s">
+        <v>228</v>
+      </c>
+      <c r="D409" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E409">
+        <v>-39.99</v>
+      </c>
+    </row>
+    <row r="410" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A410" s="5">
+        <v>44885</v>
+      </c>
+      <c r="B410" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C410" t="s">
+        <v>250</v>
+      </c>
+      <c r="D410" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E410">
+        <v>-29.63</v>
+      </c>
+    </row>
+    <row r="411" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A411" s="5">
+        <v>44886</v>
+      </c>
+      <c r="B411" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C411" t="s">
+        <v>137</v>
+      </c>
+      <c r="D411" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E411">
+        <v>-11.99</v>
+      </c>
+    </row>
+    <row r="412" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A412" s="5">
+        <v>44886</v>
+      </c>
+      <c r="B412" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C412" t="s">
+        <v>137</v>
+      </c>
+      <c r="D412" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E412" s="6">
+        <v>-24.24</v>
+      </c>
+    </row>
+    <row r="413" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A413" s="5">
+        <v>44886</v>
+      </c>
+      <c r="B413" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C413" t="s">
+        <v>137</v>
+      </c>
+      <c r="D413" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E413" s="6">
+        <v>-94.13</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A414" s="5">
+        <v>44886</v>
+      </c>
+      <c r="B414" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C414" t="s">
+        <v>137</v>
+      </c>
+      <c r="D414" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E414" s="6">
+        <v>-25.99</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A415" s="5">
+        <v>44886</v>
+      </c>
+      <c r="B415" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C415" t="s">
+        <v>57</v>
+      </c>
+      <c r="D415" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E415">
+        <v>-1218</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9062,7 +9613,7 @@
           <x14:formula1>
             <xm:f>OFFSET(Categories!$A$2,0,0,COUNTIF(Categories!$A$2:$A$99,"&lt;&gt;"))</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D384</xm:sqref>
+          <xm:sqref>D2:D415</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
weekly update corrected syntax
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffgood/Desktop/R_Studio_Projects/Financial_Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C86E5AF-DFC6-A343-BFCC-9FE6F71D6276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA46621-A19F-5947-B59E-3226C98953E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="980" windowWidth="15420" windowHeight="15800" xr2:uid="{D9F47917-7B20-384C-878F-0D08681ABD47}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="296">
   <si>
     <t>Date</t>
   </si>
@@ -836,6 +836,102 @@
   </si>
   <si>
     <t>Duck Donuts</t>
+  </si>
+  <si>
+    <t>Spring Health Receivable</t>
+  </si>
+  <si>
+    <t>Zelle Transfer from Allison Smeresky</t>
+  </si>
+  <si>
+    <t>Elaina_Pay</t>
+  </si>
+  <si>
+    <t>WEGMANS #45</t>
+  </si>
+  <si>
+    <t>BOMBAS LLC</t>
+  </si>
+  <si>
+    <t>HOBBY-LOBBY #823</t>
+  </si>
+  <si>
+    <t>OXO*INTERNATIONAL</t>
+  </si>
+  <si>
+    <t>Kindle Svcs</t>
+  </si>
+  <si>
+    <t>NAVY EXCHANGE 110282</t>
+  </si>
+  <si>
+    <t>Kindle Svcs*CT5FN6Z23    888-802-3080 WA</t>
+  </si>
+  <si>
+    <t>Kindle Svcs*1E5WI5U03    888-802-3080 WA</t>
+  </si>
+  <si>
+    <t>Kindle Svcs*PU2KP7513    888-802-3080 WA</t>
+  </si>
+  <si>
+    <t>Kindle Svcs*0D0XL03H3    888-802-3080 WA</t>
+  </si>
+  <si>
+    <t>Kindle Svcs*RX6YI8T23    888-802-3080 WA</t>
+  </si>
+  <si>
+    <t>DOLLAR TREE              MECHANICSBURGPA</t>
+  </si>
+  <si>
+    <t>IHERB IHERB.COM bA04l    IHERB.COM    CA</t>
+  </si>
+  <si>
+    <t>STARBUCKS 800-782-7282   800-782-7282 WA</t>
+  </si>
+  <si>
+    <t>ONTARIO AIRPORT          ONTARIO      CA</t>
+  </si>
+  <si>
+    <t>INK ST 1876              ONTARIO      CA</t>
+  </si>
+  <si>
+    <t>MCDONALD'S F17274        CHICAGO      IL</t>
+  </si>
+  <si>
+    <t>Koyla Indian Restaurant</t>
+  </si>
+  <si>
+    <t>COFFEE BEAN STORE # 119  RANCHO CUCAMOCA</t>
+  </si>
+  <si>
+    <t>Serranos Coronado</t>
+  </si>
+  <si>
+    <t>Panda Express</t>
+  </si>
+  <si>
+    <t>Sunoco</t>
+  </si>
+  <si>
+    <t>Plaza Azteca Mechanicsbur</t>
+  </si>
+  <si>
+    <t>MyEyeDr.</t>
+  </si>
+  <si>
+    <t>Miguels Cocina Coronado</t>
+  </si>
+  <si>
+    <t>Dunkin'</t>
+  </si>
+  <si>
+    <t>Burger Lounge Coronado</t>
+  </si>
+  <si>
+    <t>The Vitamin Shoppe</t>
+  </si>
+  <si>
+    <t>North Island Nas Comm</t>
   </si>
 </sst>
 </file>
@@ -2086,7 +2182,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1870C13B-AC88-4747-AFC0-996355F07F2B}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1870C13B-AC88-4747-AFC0-996355F07F2B}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -2205,10 +2301,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}" name="Table1" displayName="Table1" ref="A1:E435" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E435" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E435">
-    <sortCondition ref="A1:A435"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}" name="Table1" displayName="Table1" ref="A1:E488" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E488" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E488">
+    <sortCondition ref="A1:A488"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{36D6B367-4586-164A-BAFD-F61BD8D7B0D8}" name="Date" dataDxfId="4"/>
@@ -2518,10 +2614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BEBEFE-BF8C-CE41-8907-E9633ACA1DDB}">
-  <dimension ref="A1:E435"/>
+  <dimension ref="A1:E488"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D436" sqref="D436"/>
+      <selection activeCell="D444" sqref="D444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9964,6 +10060,907 @@
         <v>-15.04</v>
       </c>
     </row>
+    <row r="436" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A436" s="5">
+        <v>44893</v>
+      </c>
+      <c r="B436" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C436" t="s">
+        <v>292</v>
+      </c>
+      <c r="D436" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E436">
+        <v>-8.25</v>
+      </c>
+    </row>
+    <row r="437" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A437" s="5">
+        <v>44893</v>
+      </c>
+      <c r="B437" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C437" t="s">
+        <v>292</v>
+      </c>
+      <c r="D437" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E437">
+        <v>-11.53</v>
+      </c>
+    </row>
+    <row r="438" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A438" s="5">
+        <v>44893</v>
+      </c>
+      <c r="B438" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C438" t="s">
+        <v>234</v>
+      </c>
+      <c r="D438" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E438">
+        <v>-15.04</v>
+      </c>
+    </row>
+    <row r="439" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A439" s="5">
+        <v>44893</v>
+      </c>
+      <c r="B439" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C439" t="s">
+        <v>293</v>
+      </c>
+      <c r="D439" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E439">
+        <v>-18.88</v>
+      </c>
+    </row>
+    <row r="440" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A440" s="5">
+        <v>44893</v>
+      </c>
+      <c r="B440" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C440" t="s">
+        <v>294</v>
+      </c>
+      <c r="D440" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E440">
+        <v>-37.49</v>
+      </c>
+    </row>
+    <row r="441" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A441" s="5">
+        <v>44893</v>
+      </c>
+      <c r="B441" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C441" t="s">
+        <v>182</v>
+      </c>
+      <c r="D441" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E441">
+        <v>-64</v>
+      </c>
+    </row>
+    <row r="442" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A442" s="5">
+        <v>44893</v>
+      </c>
+      <c r="B442" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C442" t="s">
+        <v>295</v>
+      </c>
+      <c r="D442" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E442">
+        <v>-12.48</v>
+      </c>
+    </row>
+    <row r="443" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A443" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B443" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C443" t="s">
+        <v>204</v>
+      </c>
+      <c r="D443" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E443">
+        <v>-27.03</v>
+      </c>
+    </row>
+    <row r="444" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A444" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B444" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C444" t="s">
+        <v>204</v>
+      </c>
+      <c r="D444" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E444" s="6">
+        <v>-13.99</v>
+      </c>
+    </row>
+    <row r="445" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A445" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B445" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C445" t="s">
+        <v>204</v>
+      </c>
+      <c r="D445" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E445" s="6">
+        <v>-99.5</v>
+      </c>
+    </row>
+    <row r="446" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A446" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B446" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C446" t="s">
+        <v>204</v>
+      </c>
+      <c r="D446" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E446" s="6">
+        <v>-26.78</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A447" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B447" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C447" t="s">
+        <v>207</v>
+      </c>
+      <c r="D447" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E447">
+        <v>-1733.86</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A448" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B448" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C448" t="s">
+        <v>264</v>
+      </c>
+      <c r="D448" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="E448">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A449" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B449" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C449" t="s">
+        <v>265</v>
+      </c>
+      <c r="D449" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E449">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="450" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A450" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B450" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C450" t="s">
+        <v>207</v>
+      </c>
+      <c r="D450" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E450">
+        <v>1733.86</v>
+      </c>
+    </row>
+    <row r="451" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A451" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B451" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C451" t="s">
+        <v>182</v>
+      </c>
+      <c r="D451" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E451">
+        <v>-9.99</v>
+      </c>
+    </row>
+    <row r="452" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A452" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B452" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C452" t="s">
+        <v>290</v>
+      </c>
+      <c r="D452" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E452">
+        <v>-124</v>
+      </c>
+    </row>
+    <row r="453" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A453" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B453" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C453" t="s">
+        <v>213</v>
+      </c>
+      <c r="D453" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E453">
+        <v>-8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A454" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B454" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C454" t="s">
+        <v>73</v>
+      </c>
+      <c r="D454" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E454">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A455" s="5">
+        <v>44894</v>
+      </c>
+      <c r="B455" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C455" t="s">
+        <v>291</v>
+      </c>
+      <c r="D455" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E455">
+        <v>-27.71</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A456" s="5">
+        <v>44895</v>
+      </c>
+      <c r="B456" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C456" t="s">
+        <v>203</v>
+      </c>
+      <c r="D456" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E456">
+        <v>2952.87</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A457" s="5">
+        <v>44895</v>
+      </c>
+      <c r="B457" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C457" t="s">
+        <v>202</v>
+      </c>
+      <c r="D457" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E457">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A458" s="5">
+        <v>44895</v>
+      </c>
+      <c r="B458" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C458" t="s">
+        <v>272</v>
+      </c>
+      <c r="D458" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E458">
+        <v>-2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A459" s="5">
+        <v>44895</v>
+      </c>
+      <c r="B459" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C459" t="s">
+        <v>286</v>
+      </c>
+      <c r="D459" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E459">
+        <v>-27.75</v>
+      </c>
+    </row>
+    <row r="460" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A460" s="5">
+        <v>44895</v>
+      </c>
+      <c r="B460" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C460" t="s">
+        <v>287</v>
+      </c>
+      <c r="D460" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E460">
+        <v>-12.71</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A461" s="5">
+        <v>44895</v>
+      </c>
+      <c r="B461" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C461" t="s">
+        <v>288</v>
+      </c>
+      <c r="D461" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E461">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A462" s="5">
+        <v>44895</v>
+      </c>
+      <c r="B462" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C462" t="s">
+        <v>289</v>
+      </c>
+      <c r="D462" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E462">
+        <v>-21.36</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A463" s="5">
+        <v>44896</v>
+      </c>
+      <c r="B463" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C463" t="s">
+        <v>204</v>
+      </c>
+      <c r="D463" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E463">
+        <v>-22.79</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A464" s="5">
+        <v>44896</v>
+      </c>
+      <c r="B464" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C464" t="s">
+        <v>180</v>
+      </c>
+      <c r="D464" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E464">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A465" s="5">
+        <v>44896</v>
+      </c>
+      <c r="B465" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C465" t="s">
+        <v>180</v>
+      </c>
+      <c r="D465" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E465">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A466" s="5">
+        <v>44896</v>
+      </c>
+      <c r="B466" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C466" t="s">
+        <v>180</v>
+      </c>
+      <c r="D466" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E466">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="467" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A467" s="5">
+        <v>44896</v>
+      </c>
+      <c r="B467" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C467" t="s">
+        <v>284</v>
+      </c>
+      <c r="D467" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E467">
+        <v>-26.2</v>
+      </c>
+    </row>
+    <row r="468" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A468" s="5">
+        <v>44896</v>
+      </c>
+      <c r="B468" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C468" t="s">
+        <v>285</v>
+      </c>
+      <c r="D468" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E468">
+        <v>-5.15</v>
+      </c>
+    </row>
+    <row r="469" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A469" s="5">
+        <v>44897</v>
+      </c>
+      <c r="B469" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C469" t="s">
+        <v>199</v>
+      </c>
+      <c r="D469" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E469">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="470" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A470" s="5">
+        <v>44897</v>
+      </c>
+      <c r="B470" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C470" t="s">
+        <v>280</v>
+      </c>
+      <c r="D470" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E470">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="471" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A471" s="5">
+        <v>44897</v>
+      </c>
+      <c r="B471" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C471" t="s">
+        <v>281</v>
+      </c>
+      <c r="D471" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E471">
+        <v>-11.63</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A472" s="5">
+        <v>44897</v>
+      </c>
+      <c r="B472" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C472" t="s">
+        <v>282</v>
+      </c>
+      <c r="D472" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E472">
+        <v>-12.41</v>
+      </c>
+    </row>
+    <row r="473" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A473" s="5">
+        <v>44897</v>
+      </c>
+      <c r="B473" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C473" t="s">
+        <v>283</v>
+      </c>
+      <c r="D473" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E473">
+        <v>-12.82</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A474" s="5">
+        <v>44898</v>
+      </c>
+      <c r="B474" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C474" t="s">
+        <v>269</v>
+      </c>
+      <c r="D474" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E474">
+        <v>-66.92</v>
+      </c>
+    </row>
+    <row r="475" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A475" s="5">
+        <v>44898</v>
+      </c>
+      <c r="B475" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C475" t="s">
+        <v>270</v>
+      </c>
+      <c r="D475" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E475">
+        <v>-28.59</v>
+      </c>
+    </row>
+    <row r="476" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A476" s="5">
+        <v>44898</v>
+      </c>
+      <c r="B476" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C476" t="s">
+        <v>271</v>
+      </c>
+      <c r="D476" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E476">
+        <v>-10.59</v>
+      </c>
+    </row>
+    <row r="477" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A477" s="5">
+        <v>44898</v>
+      </c>
+      <c r="B477" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C477" t="s">
+        <v>273</v>
+      </c>
+      <c r="D477" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E477">
+        <v>-10.59</v>
+      </c>
+    </row>
+    <row r="478" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A478" s="5">
+        <v>44898</v>
+      </c>
+      <c r="B478" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C478" t="s">
+        <v>274</v>
+      </c>
+      <c r="D478" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E478">
+        <v>-15.89</v>
+      </c>
+    </row>
+    <row r="479" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A479" s="5">
+        <v>44898</v>
+      </c>
+      <c r="B479" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C479" t="s">
+        <v>275</v>
+      </c>
+      <c r="D479" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E479">
+        <v>-15.89</v>
+      </c>
+    </row>
+    <row r="480" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A480" s="5">
+        <v>44898</v>
+      </c>
+      <c r="B480" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C480" t="s">
+        <v>276</v>
+      </c>
+      <c r="D480" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E480">
+        <v>-10.59</v>
+      </c>
+    </row>
+    <row r="481" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A481" s="5">
+        <v>44898</v>
+      </c>
+      <c r="B481" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C481" t="s">
+        <v>277</v>
+      </c>
+      <c r="D481" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E481">
+        <v>-15.89</v>
+      </c>
+    </row>
+    <row r="482" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A482" s="5">
+        <v>44898</v>
+      </c>
+      <c r="B482" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C482" t="s">
+        <v>278</v>
+      </c>
+      <c r="D482" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E482">
+        <v>-66.709999999999994</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A483" s="5">
+        <v>44898</v>
+      </c>
+      <c r="B483" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C483" t="s">
+        <v>151</v>
+      </c>
+      <c r="D483" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E483">
+        <v>-21.68</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A484" s="5">
+        <v>44898</v>
+      </c>
+      <c r="B484" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C484" t="s">
+        <v>279</v>
+      </c>
+      <c r="D484" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E484">
+        <v>-12.47</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A485" s="5">
+        <v>44898</v>
+      </c>
+      <c r="B485" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C485" t="s">
+        <v>279</v>
+      </c>
+      <c r="D485" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E485">
+        <v>-59.81</v>
+      </c>
+    </row>
+    <row r="486" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A486" s="5">
+        <v>44899</v>
+      </c>
+      <c r="B486" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C486" t="s">
+        <v>34</v>
+      </c>
+      <c r="D486" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E486">
+        <v>-11.65</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A487" s="5">
+        <v>44899</v>
+      </c>
+      <c r="B487" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C487" t="s">
+        <v>267</v>
+      </c>
+      <c r="D487" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E487">
+        <v>-34.08</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A488" s="5">
+        <v>44899</v>
+      </c>
+      <c r="B488" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C488" t="s">
+        <v>268</v>
+      </c>
+      <c r="D488" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E488">
+        <v>-146.88</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9977,7 +10974,7 @@
           <x14:formula1>
             <xm:f>OFFSET(Categories!$A$2,0,0,COUNTIF(Categories!$A$2:$A$99,"&lt;&gt;"))</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D435</xm:sqref>
+          <xm:sqref>D2:D488</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9987,10 +10984,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A85DC7-AAE6-0D45-BE57-A2D20F484BD4}">
-  <dimension ref="A1:A38"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10055,143 +11052,148 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>229</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:A9" xr:uid="{92A85DC7-AAE6-0D45-BE57-A2D20F484BD4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A38">
-      <sortCondition ref="A1:A38"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A39">
+      <sortCondition ref="A1:A39"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Weekly update and added fixed rate loan
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffgood/Desktop/R_Studio_Projects/Financial_Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA43A75-CD90-CF44-9C68-7DA76E7CE695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868A3E80-B1A7-424A-BC13-B2CEEF097CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="980" windowWidth="15420" windowHeight="15800" xr2:uid="{D9F47917-7B20-384C-878F-0D08681ABD47}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2461" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2527" uniqueCount="368">
   <si>
     <t>Date</t>
   </si>
@@ -1135,6 +1135,15 @@
   </si>
   <si>
     <t>Auntie Anne's</t>
+  </si>
+  <si>
+    <t>IHERB IHERB.COM wtyEN</t>
+  </si>
+  <si>
+    <t>TRINDLE BOWL</t>
+  </si>
+  <si>
+    <t>ALDI 71146</t>
   </si>
 </sst>
 </file>
@@ -1213,12 +1222,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1295,10 +1304,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}" name="Table1" displayName="Table1" ref="A1:E812" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E812" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E812">
-    <sortCondition ref="A1:A812"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}" name="Table1" displayName="Table1" ref="A1:E834" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E834" xr:uid="{873B626F-84B1-204D-BA29-18F956DFEC2E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E834">
+    <sortCondition ref="A1:A834"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{36D6B367-4586-164A-BAFD-F61BD8D7B0D8}" name="Date" dataDxfId="4"/>
@@ -1608,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BEBEFE-BF8C-CE41-8907-E9633ACA1DDB}">
-  <dimension ref="A1:E812"/>
+  <dimension ref="A1:E834"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D813" sqref="D813"/>
+      <selection activeCell="D835" sqref="D835"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14903,7 +14912,7 @@
       </c>
     </row>
     <row r="780" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A780" s="3">
+      <c r="A780" s="2">
         <v>44977</v>
       </c>
       <c r="B780" t="s">
@@ -14912,7 +14921,7 @@
       <c r="C780" t="s">
         <v>161</v>
       </c>
-      <c r="D780" s="4" t="s">
+      <c r="D780" t="s">
         <v>264</v>
       </c>
       <c r="E780">
@@ -14920,7 +14929,7 @@
       </c>
     </row>
     <row r="781" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A781" s="3">
+      <c r="A781" s="2">
         <v>44977</v>
       </c>
       <c r="B781" t="s">
@@ -14929,7 +14938,7 @@
       <c r="C781" t="s">
         <v>254</v>
       </c>
-      <c r="D781" s="4" t="s">
+      <c r="D781" t="s">
         <v>264</v>
       </c>
       <c r="E781">
@@ -14988,7 +14997,7 @@
       </c>
     </row>
     <row r="785" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A785" s="3">
+      <c r="A785" s="2">
         <v>44978</v>
       </c>
       <c r="B785" t="s">
@@ -14997,7 +15006,7 @@
       <c r="C785" t="s">
         <v>364</v>
       </c>
-      <c r="D785" s="4" t="s">
+      <c r="D785" t="s">
         <v>268</v>
       </c>
       <c r="E785">
@@ -15005,7 +15014,7 @@
       </c>
     </row>
     <row r="786" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A786" s="3">
+      <c r="A786" s="2">
         <v>44978</v>
       </c>
       <c r="B786" t="s">
@@ -15014,7 +15023,7 @@
       <c r="C786" t="s">
         <v>53</v>
       </c>
-      <c r="D786" s="4" t="s">
+      <c r="D786" t="s">
         <v>54</v>
       </c>
       <c r="E786">
@@ -15022,7 +15031,7 @@
       </c>
     </row>
     <row r="787" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A787" s="3">
+      <c r="A787" s="2">
         <v>44978</v>
       </c>
       <c r="B787" t="s">
@@ -15031,7 +15040,7 @@
       <c r="C787" t="s">
         <v>282</v>
       </c>
-      <c r="D787" s="4" t="s">
+      <c r="D787" t="s">
         <v>266</v>
       </c>
       <c r="E787">
@@ -15056,7 +15065,7 @@
       </c>
     </row>
     <row r="789" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A789" s="3">
+      <c r="A789" s="2">
         <v>44979</v>
       </c>
       <c r="B789" t="s">
@@ -15065,7 +15074,7 @@
       <c r="C789" t="s">
         <v>351</v>
       </c>
-      <c r="D789" s="4" t="s">
+      <c r="D789" t="s">
         <v>310</v>
       </c>
       <c r="E789">
@@ -15073,7 +15082,7 @@
       </c>
     </row>
     <row r="790" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A790" s="3">
+      <c r="A790" s="2">
         <v>44980</v>
       </c>
       <c r="B790" t="s">
@@ -15082,7 +15091,7 @@
       <c r="C790" t="s">
         <v>160</v>
       </c>
-      <c r="D790" s="4" t="s">
+      <c r="D790" t="s">
         <v>263</v>
       </c>
       <c r="E790">
@@ -15090,7 +15099,7 @@
       </c>
     </row>
     <row r="791" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A791" s="3">
+      <c r="A791" s="2">
         <v>44980</v>
       </c>
       <c r="B791" t="s">
@@ -15099,7 +15108,7 @@
       <c r="C791" t="s">
         <v>161</v>
       </c>
-      <c r="D791" s="4" t="s">
+      <c r="D791" t="s">
         <v>264</v>
       </c>
       <c r="E791">
@@ -15107,7 +15116,7 @@
       </c>
     </row>
     <row r="792" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A792" s="3">
+      <c r="A792" s="2">
         <v>44980</v>
       </c>
       <c r="B792" t="s">
@@ -15116,7 +15125,7 @@
       <c r="C792" t="s">
         <v>363</v>
       </c>
-      <c r="D792" s="4" t="s">
+      <c r="D792" t="s">
         <v>268</v>
       </c>
       <c r="E792">
@@ -15124,16 +15133,16 @@
       </c>
     </row>
     <row r="793" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A793" s="7">
+      <c r="A793" s="5">
         <v>44981</v>
       </c>
-      <c r="B793" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C793" s="5" t="s">
+      <c r="B793" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C793" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D793" s="4" t="s">
+      <c r="D793" t="s">
         <v>263</v>
       </c>
       <c r="E793">
@@ -15141,16 +15150,16 @@
       </c>
     </row>
     <row r="794" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A794" s="7">
+      <c r="A794" s="5">
         <v>44981</v>
       </c>
-      <c r="B794" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C794" s="5" t="s">
+      <c r="B794" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C794" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="D794" s="4" t="s">
+      <c r="D794" t="s">
         <v>310</v>
       </c>
       <c r="E794">
@@ -15158,7 +15167,7 @@
       </c>
     </row>
     <row r="795" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A795" s="3">
+      <c r="A795" s="2">
         <v>44981</v>
       </c>
       <c r="B795" t="s">
@@ -15167,7 +15176,7 @@
       <c r="C795" t="s">
         <v>206</v>
       </c>
-      <c r="D795" s="4" t="s">
+      <c r="D795" t="s">
         <v>266</v>
       </c>
       <c r="E795">
@@ -15175,7 +15184,7 @@
       </c>
     </row>
     <row r="796" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A796" s="3">
+      <c r="A796" s="2">
         <v>44981</v>
       </c>
       <c r="B796" t="s">
@@ -15184,7 +15193,7 @@
       <c r="C796" t="s">
         <v>227</v>
       </c>
-      <c r="D796" s="4" t="s">
+      <c r="D796" t="s">
         <v>265</v>
       </c>
       <c r="E796">
@@ -15192,7 +15201,7 @@
       </c>
     </row>
     <row r="797" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A797" s="3">
+      <c r="A797" s="2">
         <v>44982</v>
       </c>
       <c r="B797" t="s">
@@ -15201,7 +15210,7 @@
       <c r="C797" t="s">
         <v>152</v>
       </c>
-      <c r="D797" s="4" t="s">
+      <c r="D797" t="s">
         <v>12</v>
       </c>
       <c r="E797">
@@ -15209,41 +15218,41 @@
       </c>
     </row>
     <row r="798" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A798" s="6">
+      <c r="A798" s="4">
         <v>44982</v>
       </c>
-      <c r="B798" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C798" s="8" t="s">
+      <c r="B798" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C798" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D798" s="4" t="s">
+      <c r="D798" t="s">
         <v>264</v>
       </c>
-      <c r="E798" s="4">
+      <c r="E798">
         <v>-20</v>
       </c>
     </row>
     <row r="799" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A799" s="6">
+      <c r="A799" s="4">
         <v>44982</v>
       </c>
-      <c r="B799" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C799" s="8" t="s">
+      <c r="B799" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C799" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D799" s="4" t="s">
+      <c r="D799" t="s">
         <v>265</v>
       </c>
-      <c r="E799" s="4">
+      <c r="E799">
         <v>-16.5</v>
       </c>
     </row>
     <row r="800" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A800" s="3">
+      <c r="A800" s="2">
         <v>44982</v>
       </c>
       <c r="B800" t="s">
@@ -15252,7 +15261,7 @@
       <c r="C800" t="s">
         <v>156</v>
       </c>
-      <c r="D800" s="4" t="s">
+      <c r="D800" t="s">
         <v>266</v>
       </c>
       <c r="E800">
@@ -15260,7 +15269,7 @@
       </c>
     </row>
     <row r="801" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A801" s="3">
+      <c r="A801" s="2">
         <v>44982</v>
       </c>
       <c r="B801" t="s">
@@ -15269,7 +15278,7 @@
       <c r="C801" t="s">
         <v>156</v>
       </c>
-      <c r="D801" s="4" t="s">
+      <c r="D801" t="s">
         <v>266</v>
       </c>
       <c r="E801">
@@ -15277,7 +15286,7 @@
       </c>
     </row>
     <row r="802" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A802" s="3">
+      <c r="A802" s="2">
         <v>44982</v>
       </c>
       <c r="B802" t="s">
@@ -15286,7 +15295,7 @@
       <c r="C802" t="s">
         <v>157</v>
       </c>
-      <c r="D802" s="4" t="s">
+      <c r="D802" t="s">
         <v>268</v>
       </c>
       <c r="E802">
@@ -15294,7 +15303,7 @@
       </c>
     </row>
     <row r="803" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A803" s="3">
+      <c r="A803" s="2">
         <v>44982</v>
       </c>
       <c r="B803" t="s">
@@ -15303,7 +15312,7 @@
       <c r="C803" t="s">
         <v>362</v>
       </c>
-      <c r="D803" s="4" t="s">
+      <c r="D803" t="s">
         <v>268</v>
       </c>
       <c r="E803">
@@ -15311,7 +15320,7 @@
       </c>
     </row>
     <row r="804" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A804" s="3">
+      <c r="A804" s="2">
         <v>44982</v>
       </c>
       <c r="B804" t="s">
@@ -15320,7 +15329,7 @@
       <c r="C804" t="s">
         <v>357</v>
       </c>
-      <c r="D804" s="4" t="s">
+      <c r="D804" t="s">
         <v>264</v>
       </c>
       <c r="E804">
@@ -15328,7 +15337,7 @@
       </c>
     </row>
     <row r="805" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A805" s="3">
+      <c r="A805" s="2">
         <v>44983</v>
       </c>
       <c r="B805" t="s">
@@ -15337,7 +15346,7 @@
       <c r="C805" t="s">
         <v>156</v>
       </c>
-      <c r="D805" s="4" t="s">
+      <c r="D805" t="s">
         <v>266</v>
       </c>
       <c r="E805">
@@ -15396,7 +15405,7 @@
       </c>
     </row>
     <row r="809" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A809" s="3">
+      <c r="A809" s="2">
         <v>44984</v>
       </c>
       <c r="B809" t="s">
@@ -15405,7 +15414,7 @@
       <c r="C809" t="s">
         <v>343</v>
       </c>
-      <c r="D809" s="4" t="s">
+      <c r="D809" t="s">
         <v>310</v>
       </c>
       <c r="E809">
@@ -15447,7 +15456,7 @@
       </c>
     </row>
     <row r="812" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A812" s="3">
+      <c r="A812" s="2">
         <v>44985</v>
       </c>
       <c r="B812" t="s">
@@ -15456,11 +15465,385 @@
       <c r="C812" t="s">
         <v>43</v>
       </c>
-      <c r="D812" s="4" t="s">
+      <c r="D812" t="s">
         <v>91</v>
       </c>
       <c r="E812">
         <v>3126.76</v>
+      </c>
+    </row>
+    <row r="813" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A813" s="7">
+        <v>44985</v>
+      </c>
+      <c r="B813" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C813" t="s">
+        <v>169</v>
+      </c>
+      <c r="D813" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E813">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="814" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A814" s="7">
+        <v>44985</v>
+      </c>
+      <c r="B814" t="s">
+        <v>21</v>
+      </c>
+      <c r="C814" t="s">
+        <v>200</v>
+      </c>
+      <c r="D814" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E814">
+        <v>-16.11</v>
+      </c>
+    </row>
+    <row r="815" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A815" s="7">
+        <v>44985</v>
+      </c>
+      <c r="B815" t="s">
+        <v>21</v>
+      </c>
+      <c r="C815" t="s">
+        <v>229</v>
+      </c>
+      <c r="D815" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E815">
+        <v>-9.56</v>
+      </c>
+    </row>
+    <row r="816" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A816" s="7">
+        <v>44985</v>
+      </c>
+      <c r="B816" t="s">
+        <v>21</v>
+      </c>
+      <c r="C816" t="s">
+        <v>157</v>
+      </c>
+      <c r="D816" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E816">
+        <v>-19.8</v>
+      </c>
+    </row>
+    <row r="817" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A817" s="7">
+        <v>44985</v>
+      </c>
+      <c r="B817" t="s">
+        <v>21</v>
+      </c>
+      <c r="C817" t="s">
+        <v>51</v>
+      </c>
+      <c r="D817" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E817">
+        <v>-11.55</v>
+      </c>
+    </row>
+    <row r="818" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A818" s="7">
+        <v>44985</v>
+      </c>
+      <c r="B818" t="s">
+        <v>21</v>
+      </c>
+      <c r="C818" t="s">
+        <v>53</v>
+      </c>
+      <c r="D818" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E818">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="819" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A819" s="7">
+        <v>44985</v>
+      </c>
+      <c r="B819" t="s">
+        <v>21</v>
+      </c>
+      <c r="C819" t="s">
+        <v>156</v>
+      </c>
+      <c r="D819" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E819">
+        <v>13.13</v>
+      </c>
+    </row>
+    <row r="820" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A820" s="7">
+        <v>44986</v>
+      </c>
+      <c r="B820" t="s">
+        <v>7</v>
+      </c>
+      <c r="C820" t="s">
+        <v>147</v>
+      </c>
+      <c r="D820" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E820">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="821" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A821" s="7">
+        <v>44986</v>
+      </c>
+      <c r="B821" t="s">
+        <v>7</v>
+      </c>
+      <c r="C821" t="s">
+        <v>147</v>
+      </c>
+      <c r="D821" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E821">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="822" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A822" s="7">
+        <v>44986</v>
+      </c>
+      <c r="B822" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C822" t="s">
+        <v>147</v>
+      </c>
+      <c r="D822" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E822">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="823" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A823" s="7">
+        <v>44986</v>
+      </c>
+      <c r="B823" t="s">
+        <v>21</v>
+      </c>
+      <c r="C823" t="s">
+        <v>149</v>
+      </c>
+      <c r="D823" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="E823">
+        <v>-9.99</v>
+      </c>
+    </row>
+    <row r="824" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A824" s="7">
+        <v>44986</v>
+      </c>
+      <c r="B824" t="s">
+        <v>21</v>
+      </c>
+      <c r="C824" t="s">
+        <v>351</v>
+      </c>
+      <c r="D824" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E824">
+        <v>-52.99</v>
+      </c>
+    </row>
+    <row r="825" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A825" s="7">
+        <v>44987</v>
+      </c>
+      <c r="B825" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C825" t="s">
+        <v>166</v>
+      </c>
+      <c r="D825" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E825">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="826" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A826" s="7">
+        <v>44987</v>
+      </c>
+      <c r="B826" t="s">
+        <v>21</v>
+      </c>
+      <c r="C826" t="s">
+        <v>367</v>
+      </c>
+      <c r="D826" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E826">
+        <v>-123.62</v>
+      </c>
+    </row>
+    <row r="827" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A827" s="7">
+        <v>44987</v>
+      </c>
+      <c r="B827" t="s">
+        <v>21</v>
+      </c>
+      <c r="C827" t="s">
+        <v>181</v>
+      </c>
+      <c r="D827" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E827">
+        <v>-23.1</v>
+      </c>
+    </row>
+    <row r="828" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A828" s="7">
+        <v>44987</v>
+      </c>
+      <c r="B828" t="s">
+        <v>21</v>
+      </c>
+      <c r="C828" t="s">
+        <v>51</v>
+      </c>
+      <c r="D828" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E828">
+        <v>-78.319999999999993</v>
+      </c>
+    </row>
+    <row r="829" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A829" s="7">
+        <v>44988</v>
+      </c>
+      <c r="B829" t="s">
+        <v>7</v>
+      </c>
+      <c r="C829" t="s">
+        <v>203</v>
+      </c>
+      <c r="D829" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E829">
+        <v>-120.3</v>
+      </c>
+    </row>
+    <row r="830" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A830" s="7">
+        <v>44989</v>
+      </c>
+      <c r="B830" t="s">
+        <v>21</v>
+      </c>
+      <c r="C830" t="s">
+        <v>28</v>
+      </c>
+      <c r="D830" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E830">
+        <v>-30.71</v>
+      </c>
+    </row>
+    <row r="831" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A831" s="7">
+        <v>44989</v>
+      </c>
+      <c r="B831" t="s">
+        <v>21</v>
+      </c>
+      <c r="C831" t="s">
+        <v>366</v>
+      </c>
+      <c r="D831" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E831">
+        <v>-15.75</v>
+      </c>
+    </row>
+    <row r="832" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A832" s="7">
+        <v>44989</v>
+      </c>
+      <c r="B832" t="s">
+        <v>21</v>
+      </c>
+      <c r="C832" t="s">
+        <v>366</v>
+      </c>
+      <c r="D832" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E832">
+        <v>-26.25</v>
+      </c>
+    </row>
+    <row r="833" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A833" s="7">
+        <v>44989</v>
+      </c>
+      <c r="B833" t="s">
+        <v>21</v>
+      </c>
+      <c r="C833" t="s">
+        <v>366</v>
+      </c>
+      <c r="D833" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E833">
+        <v>-9.75</v>
+      </c>
+    </row>
+    <row r="834" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A834" s="7">
+        <v>44990</v>
+      </c>
+      <c r="B834" t="s">
+        <v>21</v>
+      </c>
+      <c r="C834" t="s">
+        <v>365</v>
+      </c>
+      <c r="D834" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E834">
+        <v>-55.54</v>
       </c>
     </row>
   </sheetData>
@@ -15476,7 +15859,7 @@
           <x14:formula1>
             <xm:f>OFFSET(Categories!$A$2,0,0,COUNTIF(Categories!$A$2:$A$99,"&lt;&gt;"))</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D812</xm:sqref>
+          <xm:sqref>D2:D834</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>